<commit_message>
COrrected date for Germany example for appendix
</commit_message>
<xml_diff>
--- a/Output/AppendixTab1.xlsx
+++ b/Output/AppendixTab1.xlsx
@@ -419,19 +419,13 @@
         <v>0.006754162448951098</v>
       </c>
       <c r="D2">
-        <v>-0.0010156353076204</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.001597586765676635</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0005819514580562349</v>
-      </c>
-      <c r="G2">
-        <v>0.7329932314471945</v>
-      </c>
-      <c r="H2">
-        <v>0.2670067685528054</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -447,19 +441,19 @@
         <v>0.01227108704745637</v>
       </c>
       <c r="D3">
-        <v>-0.006532559906125669</v>
+        <v>-0.005516924598505269</v>
       </c>
       <c r="E3">
-        <v>-0.001750790084289477</v>
+        <v>5.403861845915836e-005</v>
       </c>
       <c r="F3">
-        <v>-0.004781769821836192</v>
+        <v>-0.005570963216964427</v>
       </c>
       <c r="G3">
-        <v>0.2680098015860118</v>
+        <v>0.009606862369154949</v>
       </c>
       <c r="H3">
-        <v>0.7319901984139882</v>
+        <v>0.9903931376308451</v>
       </c>
     </row>
     <row r="4">
@@ -475,19 +469,19 @@
         <v>0.01621881327039994</v>
       </c>
       <c r="D4">
-        <v>-0.01048028612906925</v>
+        <v>-0.009464650821448846</v>
       </c>
       <c r="E4">
-        <v>-0.002415362305282529</v>
+        <v>0.0004602093717535852</v>
       </c>
       <c r="F4">
-        <v>-0.008064923823786718</v>
+        <v>-0.009924860193202432</v>
       </c>
       <c r="G4">
-        <v>0.2304672101063177</v>
+        <v>0.0443145198859854</v>
       </c>
       <c r="H4">
-        <v>0.7695327898936824</v>
+        <v>0.9556854801140146</v>
       </c>
     </row>
     <row r="5">
@@ -503,19 +497,19 @@
         <v>0.01732289677803195</v>
       </c>
       <c r="D5">
-        <v>-0.01158436963670126</v>
+        <v>-0.01056873432908085</v>
       </c>
       <c r="E5">
-        <v>-0.01053342227139651</v>
+        <v>-0.00640649477880307</v>
       </c>
       <c r="F5">
-        <v>-0.00105094736530474</v>
+        <v>-0.004162239550277782</v>
       </c>
       <c r="G5">
-        <v>0.9092788474242777</v>
+        <v>0.6061742664090822</v>
       </c>
       <c r="H5">
-        <v>0.0907211525757224</v>
+        <v>0.3938257335909177</v>
       </c>
     </row>
     <row r="6">
@@ -531,19 +525,19 @@
         <v>0.02276530386775508</v>
       </c>
       <c r="D6">
-        <v>-0.01702677672642438</v>
+        <v>-0.01601114141880398</v>
       </c>
       <c r="E6">
-        <v>-0.002456581937932825</v>
+        <v>-0.0005175320192456988</v>
       </c>
       <c r="F6">
-        <v>-0.01457019478849156</v>
+        <v>-0.01549360939955828</v>
       </c>
       <c r="G6">
-        <v>0.1442775680566939</v>
+        <v>0.03232324327845191</v>
       </c>
       <c r="H6">
-        <v>0.8557224319433062</v>
+        <v>0.9676767567215481</v>
       </c>
     </row>
     <row r="7">
@@ -559,19 +553,19 @@
         <v>0.03983587515221891</v>
       </c>
       <c r="D7">
-        <v>-0.03409734801088821</v>
+        <v>-0.03308171270326781</v>
       </c>
       <c r="E7">
-        <v>-0.01864627822318112</v>
+        <v>-0.01507069312187183</v>
       </c>
       <c r="F7">
-        <v>-0.0154510697877071</v>
+        <v>-0.01801101958139599</v>
       </c>
       <c r="G7">
-        <v>0.5468542074658372</v>
+        <v>0.4555596397638488</v>
       </c>
       <c r="H7">
-        <v>0.4531457925341628</v>
+        <v>0.5444403602361511</v>
       </c>
     </row>
     <row r="8">
@@ -587,19 +581,19 @@
         <v>0.04349561395511622</v>
       </c>
       <c r="D8">
-        <v>-0.03775708681378552</v>
+        <v>-0.03674145150616512</v>
       </c>
       <c r="E8">
-        <v>-0.01935061272237569</v>
+        <v>-0.0142996188151363</v>
       </c>
       <c r="F8">
-        <v>-0.01840647409140983</v>
+        <v>-0.02244183269102882</v>
       </c>
       <c r="G8">
-        <v>0.5125028002772335</v>
+        <v>0.3891958055259972</v>
       </c>
       <c r="H8">
-        <v>0.4874971997227665</v>
+        <v>0.6108041944740028</v>
       </c>
     </row>
     <row r="9">
@@ -615,19 +609,19 @@
         <v>0.08615529080345091</v>
       </c>
       <c r="D9">
-        <v>-0.08041676366212021</v>
+        <v>-0.07940112835449982</v>
       </c>
       <c r="E9">
-        <v>-0.03720806206325921</v>
+        <v>-0.03089001912198475</v>
       </c>
       <c r="F9">
-        <v>-0.043208701598861</v>
+        <v>-0.04851110923251507</v>
       </c>
       <c r="G9">
-        <v>0.462690369132398</v>
+        <v>0.3890375333719569</v>
       </c>
       <c r="H9">
-        <v>0.537309630867602</v>
+        <v>0.6109624666280432</v>
       </c>
     </row>
     <row r="10">
@@ -643,19 +637,19 @@
         <v>0.1063320056230004</v>
       </c>
       <c r="D10">
-        <v>-0.1005934784816697</v>
+        <v>-0.0995778431740493</v>
       </c>
       <c r="E10">
-        <v>-0.04713292416371606</v>
+        <v>-0.04091651535933921</v>
       </c>
       <c r="F10">
-        <v>-0.05346055431795363</v>
+        <v>-0.05866132781471008</v>
       </c>
       <c r="G10">
-        <v>0.4685485070715066</v>
+        <v>0.4108997951263355</v>
       </c>
       <c r="H10">
-        <v>0.5314514929284934</v>
+        <v>0.5891002048736646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to figures
</commit_message>
<xml_diff>
--- a/Output/AppendixTab1.xlsx
+++ b/Output/AppendixTab1.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,247 +409,89 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>SouthKorea</t>
         </is>
       </c>
       <c r="B2" s="2">
-        <v>43919</v>
+        <v>43942</v>
       </c>
       <c r="C2">
-        <v>0.006754162448951098</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+        <v>0.02218477955630441</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>USA_NYC</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B3" s="2">
-        <v>43914</v>
+        <v>43872</v>
       </c>
       <c r="C3">
-        <v>0.01227108704745637</v>
-      </c>
-      <c r="D3">
-        <v>-0.005516924598505269</v>
-      </c>
-      <c r="E3">
-        <v>5.403861845915836e-005</v>
-      </c>
-      <c r="F3">
-        <v>-0.005570963216964427</v>
-      </c>
-      <c r="G3">
-        <v>0.009606862369154949</v>
-      </c>
-      <c r="H3">
-        <v>0.9903931376308451</v>
+        <v>0.02290025071633238</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SouthKorea</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B4" s="2">
-        <v>43921</v>
+        <v>43914</v>
       </c>
       <c r="C4">
-        <v>0.01642874167860543</v>
-      </c>
-      <c r="D4">
-        <v>-0.009674579229654335</v>
-      </c>
-      <c r="E4">
-        <v>0.0004482976730251574</v>
-      </c>
-      <c r="F4">
-        <v>-0.01012287690267949</v>
-      </c>
-      <c r="G4">
-        <v>0.0424075555478446</v>
-      </c>
-      <c r="H4">
-        <v>0.9575924444521555</v>
+        <v>0.03983587515221891</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B5" s="2">
-        <v>43906</v>
+        <v>43940</v>
       </c>
       <c r="C5">
-        <v>0.01732289677803195</v>
-      </c>
-      <c r="D5">
-        <v>-0.01056873432908085</v>
-      </c>
-      <c r="E5">
-        <v>-0.00640649477880307</v>
-      </c>
-      <c r="F5">
-        <v>-0.004162239550277782</v>
-      </c>
-      <c r="G5">
-        <v>0.6061742664090822</v>
-      </c>
-      <c r="H5">
-        <v>0.3938257335909177</v>
+        <v>0.06870385174884934</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B6" s="2">
-        <v>43872</v>
+        <v>43937</v>
       </c>
       <c r="C6">
-        <v>0.02276530386775508</v>
-      </c>
-      <c r="D6">
-        <v>-0.01601114141880398</v>
-      </c>
-      <c r="E6">
-        <v>-0.0005175320192456988</v>
-      </c>
-      <c r="F6">
-        <v>-0.01549360939955828</v>
-      </c>
-      <c r="G6">
-        <v>0.03232324327845191</v>
-      </c>
-      <c r="H6">
-        <v>0.9676767567215481</v>
+        <v>0.1050210003716739</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B7" s="2">
-        <v>43914</v>
+        <v>43941</v>
       </c>
       <c r="C7">
-        <v>0.03983587515221891</v>
-      </c>
-      <c r="D7">
-        <v>-0.03308171270326781</v>
-      </c>
-      <c r="E7">
-        <v>-0.01507069312187183</v>
-      </c>
-      <c r="F7">
-        <v>-0.01801101958139599</v>
-      </c>
-      <c r="G7">
-        <v>0.4555596397638488</v>
-      </c>
-      <c r="H7">
-        <v>0.5444403602361511</v>
+        <v>0.1272752828730058</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>USA_WA</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B8" s="2">
-        <v>43919</v>
-      </c>
-      <c r="C8">
-        <v>0.04349561395511622</v>
-      </c>
-      <c r="D8">
-        <v>-0.03674145150616512</v>
-      </c>
-      <c r="E8">
-        <v>-0.0142996188151363</v>
-      </c>
-      <c r="F8">
-        <v>-0.02244183269102882</v>
-      </c>
-      <c r="G8">
-        <v>0.3891958055259972</v>
-      </c>
-      <c r="H8">
-        <v>0.6108041944740028</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B9" s="2">
-        <v>43920</v>
-      </c>
-      <c r="C9">
-        <v>0.08673226219854474</v>
-      </c>
-      <c r="D9">
-        <v>-0.07997809974959365</v>
-      </c>
-      <c r="E9">
-        <v>-0.03125864153863288</v>
-      </c>
-      <c r="F9">
-        <v>-0.04871945821096077</v>
-      </c>
-      <c r="G9">
-        <v>0.3908400129098053</v>
-      </c>
-      <c r="H9">
-        <v>0.6091599870901947</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="B10" s="2">
-        <v>43920</v>
-      </c>
-      <c r="C10">
-        <v>0.1063067266095513</v>
-      </c>
-      <c r="D10">
-        <v>-0.09955256416060018</v>
-      </c>
-      <c r="E10">
-        <v>-0.03982607333667873</v>
-      </c>
-      <c r="F10">
-        <v>-0.05972649082392145</v>
-      </c>
-      <c r="G10">
-        <v>0.400050703590422</v>
-      </c>
-      <c r="H10">
-        <v>0.5999492964095781</v>
+        <v>43941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slightly changed code for analysis, updated results
</commit_message>
<xml_diff>
--- a/Output/AppendixTab1.xlsx
+++ b/Output/AppendixTab1.xlsx
@@ -355,13 +355,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -372,35 +372,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>CFR2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>DiffDE</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>AgeCompDE</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>RateCompDE</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>relAgeDE</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>relRateDE</t>
         </is>
@@ -409,89 +414,259 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SouthKorea</t>
-        </is>
-      </c>
-      <c r="B2" s="2">
-        <v>43942</v>
-      </c>
-      <c r="C2">
-        <v>0.02218477955630441</v>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C2" s="2">
+        <v>43906</v>
+      </c>
+      <c r="D2">
+        <v>0.01796725060231124</v>
+      </c>
+      <c r="E2">
+        <v>0.01408418784366104</v>
+      </c>
+      <c r="F2">
+        <v>-0.004529216959880018</v>
+      </c>
+      <c r="G2">
+        <v>0.01861340480354106</v>
+      </c>
+      <c r="H2">
+        <v>0.1957088961735027</v>
+      </c>
+      <c r="I2">
+        <v>0.8042911038264974</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>China</t>
-        </is>
-      </c>
-      <c r="B3" s="2">
-        <v>43872</v>
-      </c>
-      <c r="C3">
-        <v>0.02290025071633238</v>
+          <t>SouthKorea</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C3" s="2">
+        <v>43943</v>
+      </c>
+      <c r="D3">
+        <v>0.02225547035720965</v>
+      </c>
+      <c r="E3">
+        <v>0.009795968088762631</v>
+      </c>
+      <c r="F3">
+        <v>0.01243792488709594</v>
+      </c>
+      <c r="G3">
+        <v>-0.002641956798333309</v>
+      </c>
+      <c r="H3">
+        <v>0.8248025512769064</v>
+      </c>
+      <c r="I3">
+        <v>0.1751974487230937</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="B4" s="2">
-        <v>43914</v>
-      </c>
-      <c r="C4">
-        <v>0.03983587515221891</v>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C4" s="2">
+        <v>43872</v>
+      </c>
+      <c r="D4">
+        <v>0.02290025071633238</v>
+      </c>
+      <c r="E4">
+        <v>0.009151187729639902</v>
+      </c>
+      <c r="F4">
+        <v>0.007221859156972936</v>
+      </c>
+      <c r="G4">
+        <v>0.001929328572666963</v>
+      </c>
+      <c r="H4">
+        <v>0.7891717851642323</v>
+      </c>
+      <c r="I4">
+        <v>0.2108282148357678</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="B5" s="2">
-        <v>43940</v>
-      </c>
-      <c r="C5">
-        <v>0.06870385174884934</v>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C5" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D5">
+        <v>0.03205143844597228</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B6" s="2">
-        <v>43937</v>
-      </c>
-      <c r="C6">
-        <v>0.1050210003716739</v>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C6" s="2">
+        <v>43914</v>
+      </c>
+      <c r="D6">
+        <v>0.03983587515221891</v>
+      </c>
+      <c r="E6">
+        <v>-0.007784436706246629</v>
+      </c>
+      <c r="F6">
+        <v>-0.001800858098157913</v>
+      </c>
+      <c r="G6">
+        <v>-0.005983578608088725</v>
+      </c>
+      <c r="H6">
+        <v>0.2313408363527204</v>
+      </c>
+      <c r="I6">
+        <v>0.7686591636472796</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="B7" s="2">
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NYC</t>
+        </is>
+      </c>
+      <c r="C7" s="2">
         <v>43941</v>
       </c>
-      <c r="C7">
-        <v>0.1272752828730058</v>
+      <c r="D7">
+        <v>0.0708957990420689</v>
+      </c>
+      <c r="E7">
+        <v>-0.03884436059609662</v>
+      </c>
+      <c r="F7">
+        <v>0.00714009319979759</v>
+      </c>
+      <c r="G7">
+        <v>-0.04598445379589421</v>
+      </c>
+      <c r="H7">
+        <v>0.1344029004214686</v>
+      </c>
+      <c r="I7">
+        <v>0.8655970995785315</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B8" s="2">
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C8" s="2">
+        <v>43937</v>
+      </c>
+      <c r="D8">
+        <v>0.1050210003716739</v>
+      </c>
+      <c r="E8">
+        <v>-0.07296956192570159</v>
+      </c>
+      <c r="F8">
+        <v>-0.0331076802397085</v>
+      </c>
+      <c r="G8">
+        <v>-0.0398618816859931</v>
+      </c>
+      <c r="H8">
+        <v>0.4537190489565924</v>
+      </c>
+      <c r="I8">
+        <v>0.5462809510434077</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C9" s="2">
         <v>43941</v>
+      </c>
+      <c r="D9">
+        <v>0.1272752828730058</v>
+      </c>
+      <c r="E9">
+        <v>-0.09522384442703355</v>
+      </c>
+      <c r="F9">
+        <v>-0.04483297587587955</v>
+      </c>
+      <c r="G9">
+        <v>-0.050390868551154</v>
+      </c>
+      <c r="H9">
+        <v>0.4708166966545168</v>
+      </c>
+      <c r="I9">
+        <v>0.5291833033454833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results to April 22, removed France, changed file names of output
</commit_message>
<xml_diff>
--- a/Output/AppendixTab1.xlsx
+++ b/Output/AppendixTab1.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +414,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>SouthKorea</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -423,31 +423,25 @@
         </is>
       </c>
       <c r="C2" s="2">
-        <v>43906</v>
+        <v>43943</v>
       </c>
       <c r="D2">
-        <v>0.01796725060231124</v>
+        <v>0.02226482139517487</v>
       </c>
       <c r="E2">
-        <v>0.01408418784366104</v>
+        <v>-0.02226482139517487</v>
       </c>
       <c r="F2">
-        <v>-0.004529216959880018</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.01861340480354106</v>
-      </c>
-      <c r="H2">
-        <v>0.1957088961735027</v>
-      </c>
-      <c r="I2">
-        <v>0.8042911038264974</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SouthKorea</t>
+          <t>China</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -456,31 +450,25 @@
         </is>
       </c>
       <c r="C3" s="2">
-        <v>43943</v>
+        <v>43872</v>
       </c>
       <c r="D3">
-        <v>0.02225547035720965</v>
+        <v>0.02290025071633238</v>
       </c>
       <c r="E3">
-        <v>0.009795968088762631</v>
+        <v>-0.02290025071633238</v>
       </c>
       <c r="F3">
-        <v>0.01243792488709594</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-0.002641956798333309</v>
-      </c>
-      <c r="H3">
-        <v>0.8248025512769064</v>
-      </c>
-      <c r="I3">
-        <v>0.1751974487230937</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -489,31 +477,25 @@
         </is>
       </c>
       <c r="C4" s="2">
-        <v>43872</v>
+        <v>43943</v>
       </c>
       <c r="D4">
-        <v>0.02290025071633238</v>
+        <v>0.03807511017180802</v>
       </c>
       <c r="E4">
-        <v>0.009151187729639902</v>
+        <v>-0.03807511017180802</v>
       </c>
       <c r="F4">
-        <v>0.007221859156972936</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.001929328572666963</v>
-      </c>
-      <c r="H4">
-        <v>0.7891717851642323</v>
-      </c>
-      <c r="I4">
-        <v>0.2108282148357678</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -522,13 +504,13 @@
         </is>
       </c>
       <c r="C5" s="2">
-        <v>43941</v>
+        <v>43943</v>
       </c>
       <c r="D5">
-        <v>0.03205143844597228</v>
+        <v>0.05598346774242222</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-0.05598346774242222</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -540,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -549,124 +531,46 @@
         </is>
       </c>
       <c r="C6" s="2">
-        <v>43914</v>
+        <v>43943</v>
       </c>
       <c r="D6">
-        <v>0.03983587515221891</v>
+        <v>0.1040122728013148</v>
       </c>
       <c r="E6">
-        <v>-0.007784436706246629</v>
+        <v>-0.1040122728013148</v>
       </c>
       <c r="F6">
-        <v>-0.001800858098157913</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-0.005983578608088725</v>
-      </c>
-      <c r="H6">
-        <v>0.2313408363527204</v>
-      </c>
-      <c r="I6">
-        <v>0.7686591636472796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NYC</t>
+          <t>All</t>
         </is>
       </c>
       <c r="C7" s="2">
-        <v>43941</v>
+        <v>43943</v>
       </c>
       <c r="D7">
-        <v>0.0708957990420689</v>
+        <v>0.1300063316640764</v>
       </c>
       <c r="E7">
-        <v>-0.03884436059609662</v>
+        <v>-0.1300063316640764</v>
       </c>
       <c r="F7">
-        <v>0.00714009319979759</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>-0.04598445379589421</v>
-      </c>
-      <c r="H7">
-        <v>0.1344029004214686</v>
-      </c>
-      <c r="I7">
-        <v>0.8655970995785315</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="C8" s="2">
-        <v>43937</v>
-      </c>
-      <c r="D8">
-        <v>0.1050210003716739</v>
-      </c>
-      <c r="E8">
-        <v>-0.07296956192570159</v>
-      </c>
-      <c r="F8">
-        <v>-0.0331076802397085</v>
-      </c>
-      <c r="G8">
-        <v>-0.0398618816859931</v>
-      </c>
-      <c r="H8">
-        <v>0.4537190489565924</v>
-      </c>
-      <c r="I8">
-        <v>0.5462809510434077</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-      <c r="C9" s="2">
-        <v>43941</v>
-      </c>
-      <c r="D9">
-        <v>0.1272752828730058</v>
-      </c>
-      <c r="E9">
-        <v>-0.09522384442703355</v>
-      </c>
-      <c r="F9">
-        <v>-0.04483297587587955</v>
-      </c>
-      <c r="G9">
-        <v>-0.050390868551154</v>
-      </c>
-      <c r="H9">
-        <v>0.4708166966545168</v>
-      </c>
-      <c r="I9">
-        <v>0.5291833033454833</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated analysis, re-structured files
</commit_message>
<xml_diff>
--- a/Output/AppendixTab1.xlsx
+++ b/Output/AppendixTab1.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,10 +426,10 @@
         <v>43943</v>
       </c>
       <c r="D2">
-        <v>0.02226482139517487</v>
+        <v>0.02225547035720965</v>
       </c>
       <c r="E2">
-        <v>-0.02226482139517487</v>
+        <v>-0.02225547035720965</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -507,10 +507,10 @@
         <v>43943</v>
       </c>
       <c r="D5">
-        <v>0.05598346774242222</v>
+        <v>0.0559832330827703</v>
       </c>
       <c r="E5">
-        <v>-0.05598346774242222</v>
+        <v>-0.0559832330827703</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -522,22 +522,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>NYC</t>
         </is>
       </c>
       <c r="C6" s="2">
         <v>43943</v>
       </c>
       <c r="D6">
-        <v>0.1040122728013148</v>
+        <v>0.07258978752642781</v>
       </c>
       <c r="E6">
-        <v>-0.1040122728013148</v>
+        <v>-0.07258978752642781</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -549,7 +549,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -561,15 +561,42 @@
         <v>43943</v>
       </c>
       <c r="D7">
-        <v>0.1300063316640764</v>
+        <v>0.1040126934054379</v>
       </c>
       <c r="E7">
-        <v>-0.1300063316640764</v>
+        <v>-0.1040126934054379</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="C8" s="2">
+        <v>43943</v>
+      </c>
+      <c r="D8">
+        <v>0.1300061819994451</v>
+      </c>
+      <c r="E8">
+        <v>-0.1300061819994451</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated results; added file to automatically update input data; excess mortality; other minor updates
</commit_message>
<xml_diff>
--- a/Output/AppendixTab1.xlsx
+++ b/Output/AppendixTab1.xlsx
@@ -414,7 +414,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SouthKorea</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -423,25 +423,25 @@
         </is>
       </c>
       <c r="C2" s="2">
-        <v>43943</v>
+        <v>44012</v>
       </c>
       <c r="D2">
-        <v>0.02225547035720965</v>
+        <v>0.02203125</v>
       </c>
       <c r="E2">
-        <v>0.01581963981459837</v>
+        <v>0.02438820524453683</v>
       </c>
       <c r="F2">
-        <v>0.01392785055554586</v>
+        <v>0.01820958489448707</v>
       </c>
       <c r="G2">
-        <v>0.00189178925905251</v>
+        <v>0.00617862035004976</v>
       </c>
       <c r="H2">
-        <v>0.8804151496984927</v>
+        <v>0.7466553898453096</v>
       </c>
       <c r="I2">
-        <v>0.1195848503015073</v>
+        <v>0.2533446101546905</v>
       </c>
     </row>
     <row r="3">
@@ -459,22 +459,22 @@
         <v>43872</v>
       </c>
       <c r="D3">
-        <v>0.02290025071633238</v>
+        <v>0.02290248925501433</v>
       </c>
       <c r="E3">
-        <v>0.01517485945547564</v>
+        <v>0.0235169659895225</v>
       </c>
       <c r="F3">
-        <v>0.008414815462550778</v>
+        <v>0.01109164660972722</v>
       </c>
       <c r="G3">
-        <v>0.006760043992924862</v>
+        <v>0.01242531937979528</v>
       </c>
       <c r="H3">
-        <v>0.5545234529018592</v>
+        <v>0.4716444550997299</v>
       </c>
       <c r="I3">
-        <v>0.4454765470981409</v>
+        <v>0.52835554490027</v>
       </c>
     </row>
     <row r="4">
@@ -489,10 +489,10 @@
         </is>
       </c>
       <c r="C4" s="2">
-        <v>43943</v>
+        <v>44012</v>
       </c>
       <c r="D4">
-        <v>0.03807511017180802</v>
+        <v>0.04641945524453683</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -516,25 +516,25 @@
         </is>
       </c>
       <c r="C5" s="2">
-        <v>43943</v>
+        <v>44009</v>
       </c>
       <c r="D5">
-        <v>0.0559832330827703</v>
+        <v>0.04752702796222197</v>
       </c>
       <c r="E5">
-        <v>-0.01790812291096228</v>
+        <v>-0.001107572717685142</v>
       </c>
       <c r="F5">
-        <v>0.0001694370541170637</v>
+        <v>0.007542255352947743</v>
       </c>
       <c r="G5">
-        <v>-0.01807755996507934</v>
+        <v>-0.008649828070632882</v>
       </c>
       <c r="H5">
-        <v>0.009285750084729594</v>
+        <v>0.4657989435728767</v>
       </c>
       <c r="I5">
-        <v>0.9907142499152705</v>
+        <v>0.5342010564271233</v>
       </c>
     </row>
     <row r="6">
@@ -549,25 +549,25 @@
         </is>
       </c>
       <c r="C6" s="2">
-        <v>43943</v>
+        <v>44012</v>
       </c>
       <c r="D6">
-        <v>0.07258978752642781</v>
+        <v>0.08719684220304529</v>
       </c>
       <c r="E6">
-        <v>-0.03451467735461979</v>
+        <v>-0.04077738695850846</v>
       </c>
       <c r="F6">
-        <v>0.008225298647550419</v>
+        <v>0.007840018472217361</v>
       </c>
       <c r="G6">
-        <v>-0.04273997600217021</v>
+        <v>-0.04861740543072583</v>
       </c>
       <c r="H6">
-        <v>0.1613902545229491</v>
+        <v>0.1388660326708363</v>
       </c>
       <c r="I6">
-        <v>0.8386097454770508</v>
+        <v>0.8611339673291638</v>
       </c>
     </row>
     <row r="7">
@@ -582,25 +582,25 @@
         </is>
       </c>
       <c r="C7" s="2">
-        <v>43943</v>
+        <v>43972</v>
       </c>
       <c r="D7">
-        <v>0.1040126934054379</v>
+        <v>0.121913536873179</v>
       </c>
       <c r="E7">
-        <v>-0.06593758323362986</v>
+        <v>-0.07549408162864213</v>
       </c>
       <c r="F7">
-        <v>-0.03503196203454149</v>
+        <v>-0.05133669685010826</v>
       </c>
       <c r="G7">
-        <v>-0.03090562119908837</v>
+        <v>-0.02415738477853388</v>
       </c>
       <c r="H7">
-        <v>0.5312897488283176</v>
+        <v>0.6800095549560449</v>
       </c>
       <c r="I7">
-        <v>0.4687102511716825</v>
+        <v>0.3199904450439552</v>
       </c>
     </row>
     <row r="8">
@@ -615,25 +615,25 @@
         </is>
       </c>
       <c r="C8" s="2">
-        <v>43943</v>
+        <v>44012</v>
       </c>
       <c r="D8">
-        <v>0.1300061819994451</v>
+        <v>0.1403006799609075</v>
       </c>
       <c r="E8">
-        <v>-0.09193107182763709</v>
+        <v>-0.09388122471637062</v>
       </c>
       <c r="F8">
-        <v>-0.0486701250572603</v>
+        <v>-0.05876468611030111</v>
       </c>
       <c r="G8">
-        <v>-0.04326094677037679</v>
+        <v>-0.0351165386060695</v>
       </c>
       <c r="H8">
-        <v>0.5294197499242979</v>
+        <v>0.6259471612970338</v>
       </c>
       <c r="I8">
-        <v>0.4705802500757021</v>
+        <v>0.3740528387029662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>